<commit_message>
TLWP-845 - Add columns to pipeline report
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application/Templates/PipelineOpportunitiesReportTemplate.xlsx
+++ b/src/Sfa.Tl.Matching.Application/Templates/PipelineOpportunitiesReportTemplate.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Esfa\matching-basket\tl-matching\src\Sfa.Tl.Matching.Application\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7510C62-CF9E-4541-9949-6AACAFB4BD73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D056C5D-BD75-4994-B383-87D627E02E51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3240" yWindow="-14430" windowWidth="19365" windowHeight="11430" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opportunities with providers" sheetId="1" r:id="rId1"/>
     <sheet name="Opportunities with no providers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Provider name</t>
   </si>
@@ -47,6 +52,24 @@
   </si>
   <si>
     <t>Provider venue town and postcode</t>
+  </si>
+  <si>
+    <t>Provider contact name</t>
+  </si>
+  <si>
+    <t>Provider contact email</t>
+  </si>
+  <si>
+    <t>Provider contact telephone</t>
+  </si>
+  <si>
+    <t>Secondary contact name</t>
+  </si>
+  <si>
+    <t>Secondary contact email</t>
+  </si>
+  <si>
+    <t>Secondary contact telephone</t>
   </si>
 </sst>
 </file>
@@ -647,24 +670,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.6875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8125" style="1"/>
+    <col min="6" max="6" width="25.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -682,6 +711,24 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -697,28 +744,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.3125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.8125" style="3"/>
+    <col min="1" max="1" width="30.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.25" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TLWP-861 - Fix issue with loading spreadhsheet
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application/Templates/PipelineOpportunitiesReportTemplate.xlsx
+++ b/src/Sfa.Tl.Matching.Application/Templates/PipelineOpportunitiesReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Esfa\matching-basket\tl-matching\src\Sfa.Tl.Matching.Application\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D056C5D-BD75-4994-B383-87D627E02E51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF82FD01-3815-41BF-8156-F77ED7C5366C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TLWP-862 - Update opportunities report template
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application/Templates/PipelineOpportunitiesReportTemplate.xlsx
+++ b/src/Sfa.Tl.Matching.Application/Templates/PipelineOpportunitiesReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Esfa\matching-basket\tl-matching\src\Sfa.Tl.Matching.Application\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF82FD01-3815-41BF-8156-F77ED7C5366C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF66CC09-7BA5-4818-A58D-C17A9B09545E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,15 +54,6 @@
     <t>Provider venue town and postcode</t>
   </si>
   <si>
-    <t>Provider contact name</t>
-  </si>
-  <si>
-    <t>Provider contact email</t>
-  </si>
-  <si>
-    <t>Provider contact telephone</t>
-  </si>
-  <si>
     <t>Secondary contact name</t>
   </si>
   <si>
@@ -70,6 +61,15 @@
   </si>
   <si>
     <t>Secondary contact telephone</t>
+  </si>
+  <si>
+    <t>Primary contact name</t>
+  </si>
+  <si>
+    <t>Primary contact email</t>
+  </si>
+  <si>
+    <t>Primary contact telephone</t>
   </si>
 </sst>
 </file>
@@ -672,9 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -713,22 +711,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>